<commit_message>
Changes for Excel sheet
</commit_message>
<xml_diff>
--- a/EvoTax.1099/wwwroot/Templates/Form1099_G_Template.xlsx
+++ b/EvoTax.1099/wwwroot/Templates/Form1099_G_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Code Repos\EvoTaxes\EvoTax.1099\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8F0873-AF37-433B-BE4B-DA5DC5249B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E096BA-35FB-4B59-9E8B-EA71B5A9A4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,9 +458,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Is Corrected</t>
-  </si>
-  <si>
     <t>Company</t>
   </si>
   <si>
@@ -477,6 +474,9 @@
   </si>
   <si>
     <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Is Corrected Form of 1099</t>
   </si>
 </sst>
 </file>
@@ -1113,6 +1113,7 @@
     <xf numFmtId="49" fontId="22" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -1143,7 +1144,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2:AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1507,13 +1507,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1522,10 +1522,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>3</v>
@@ -1534,13 +1534,13 @@
         <v>4</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="23" t="s">
-        <v>151</v>
+      <c r="M1" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>7</v>
@@ -1597,7 +1597,7 @@
         <v>23</v>
       </c>
       <c r="AF1" s="10" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
@@ -2256,7 +2256,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576 X1:X1048576 AF1:AF13" xr:uid="{04988C7D-CC0E-46A2-A20F-F217EB9B8932}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576 X1:X1048576 AF1:AF1048576" xr:uid="{04988C7D-CC0E-46A2-A20F-F217EB9B8932}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2281,198 +2281,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>